<commit_message>
Backup QR Scanner data - 4/5/2025, 9:52:30 PM
</commit_message>
<xml_diff>
--- a/backups/qr_scanner_backup_20250405_2152.xlsx
+++ b/backups/qr_scanner_backup_20250405_2152.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Dihdhdh" sheetId="6" r:id="rId6"/>
     <sheet name="Dihdhdhusudhdh" sheetId="7" r:id="rId7"/>
     <sheet name="Mazin" sheetId="8" r:id="rId8"/>
+    <sheet name="Mazinjsbdb" sheetId="9" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -852,4 +853,52 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Student ID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Log Date</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Log Time</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Mazinjsbdb</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E2" t="str">
+        <v>21:52:27</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 4/5/2025, 9:52:50 PM
</commit_message>
<xml_diff>
--- a/backups/qr_scanner_backup_20250405_2152.xlsx
+++ b/backups/qr_scanner_backup_20250405_2152.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Dihdhdhusudhdh" sheetId="7" r:id="rId7"/>
     <sheet name="Mazin" sheetId="8" r:id="rId8"/>
     <sheet name="Mazinjsbdb" sheetId="9" r:id="rId9"/>
+    <sheet name="Mazinjsbdbmsndbd" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -451,6 +452,105 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Student ID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Log Date</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Log Time</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Mazinjsbdbmsndbd</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E2" t="str">
+        <v>21:52:35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Mazinjsbdbmsndbd</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E3" t="str">
+        <v>21:52:39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Mazinjsbdbmsndbd</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E4" t="str">
+        <v>21:52:42</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Mazinjsbdbmsndbd</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E5" t="str">
+        <v>21:52:45</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>

</xml_diff>